<commit_message>
sample output and class reclarify
</commit_message>
<xml_diff>
--- a/Data/MR_p_Data.xlsx
+++ b/Data/MR_p_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/summersane/Desktop/RA/Radiology/Example_plots_tex/ROC/Plotting/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/summersane/Desktop/RA/Radiology/Example_plots_tex/ROC/ROC_Analysis_Tex/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF02339-B063-4C48-ABA6-40DE44D34067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A17BDD1-BBB3-BC47-A43F-D04CA41EBB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19440" firstSheet="3" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19440" firstSheet="3" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,13 @@
     <sheet name="W" sheetId="22" r:id="rId22"/>
     <sheet name="X" sheetId="23" r:id="rId23"/>
     <sheet name="Y" sheetId="24" r:id="rId24"/>
-    <sheet name="Z" sheetId="26" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10100" uniqueCount="6930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9696" uniqueCount="6930">
   <si>
     <t>AUC</t>
   </si>
@@ -47262,7 +47261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -48887,1638 +48886,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7D5AB6-CF8F-164F-A8CF-D71A312CA19C}">
-  <dimension ref="A1:B202"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6747</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6748</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>3088</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2492</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>5342</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6067</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>802</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3090</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>5344</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6749</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>4521</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>1518</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2498</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>5346</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>431</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>2199</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3963</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>5349</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6750</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>5351</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6751</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>5353</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>2502</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4532</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>5355</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3970</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>2212</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6752</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>5358</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6753</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>5360</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6754</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>456</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6755</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>5362</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4539</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>5364</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6756</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>2224</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6757</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>2226</v>
-      </c>
-      <c r="B27" t="s">
-        <v>6758</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>6759</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4832</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>6760</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4834</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>6761</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4835</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>3719</v>
-      </c>
-      <c r="B31" t="s">
-        <v>4550</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>2236</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>2238</v>
-      </c>
-      <c r="B33" t="s">
-        <v>6762</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>2240</v>
-      </c>
-      <c r="B34" t="s">
-        <v>6763</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>3125</v>
-      </c>
-      <c r="B35" t="s">
-        <v>6764</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>3126</v>
-      </c>
-      <c r="B36" t="s">
-        <v>6765</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>3128</v>
-      </c>
-      <c r="B37" t="s">
-        <v>6766</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B38" t="s">
-        <v>4561</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>880</v>
-      </c>
-      <c r="B39" t="s">
-        <v>6767</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>2529</v>
-      </c>
-      <c r="B40" t="s">
-        <v>6768</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>2254</v>
-      </c>
-      <c r="B41" t="s">
-        <v>6769</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>3134</v>
-      </c>
-      <c r="B42" t="s">
-        <v>6770</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>3136</v>
-      </c>
-      <c r="B43" t="s">
-        <v>6771</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>1945</v>
-      </c>
-      <c r="B44" t="s">
-        <v>6772</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>3139</v>
-      </c>
-      <c r="B45" t="s">
-        <v>4572</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>156</v>
-      </c>
-      <c r="B46" t="s">
-        <v>2251</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
-        <v>6773</v>
-      </c>
-      <c r="B47" t="s">
-        <v>6774</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
-        <v>1572</v>
-      </c>
-      <c r="B48" t="s">
-        <v>6775</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>6776</v>
-      </c>
-      <c r="B49" t="s">
-        <v>6777</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>2269</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6778</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B51" t="s">
-        <v>6779</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>1254</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6780</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B53" t="s">
-        <v>6781</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>1258</v>
-      </c>
-      <c r="B54" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B55" t="s">
-        <v>4869</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
-        <v>1262</v>
-      </c>
-      <c r="B56" t="s">
-        <v>6782</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
-        <v>524</v>
-      </c>
-      <c r="B57" t="s">
-        <v>5392</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
-        <v>1265</v>
-      </c>
-      <c r="B58" t="s">
-        <v>5393</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B59" t="s">
-        <v>6783</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1939</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B61" t="s">
-        <v>6784</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B62" t="s">
-        <v>6785</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B63" t="s">
-        <v>6786</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
-        <v>1277</v>
-      </c>
-      <c r="B64" t="s">
-        <v>3457</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
-        <v>1597</v>
-      </c>
-      <c r="B65" t="s">
-        <v>6787</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
-        <v>540</v>
-      </c>
-      <c r="B66" t="s">
-        <v>6788</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B67" t="s">
-        <v>6789</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
-        <v>6790</v>
-      </c>
-      <c r="B68" t="s">
-        <v>6791</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
-        <v>6792</v>
-      </c>
-      <c r="B69" t="s">
-        <v>6793</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
-        <v>1288</v>
-      </c>
-      <c r="B70" t="s">
-        <v>6592</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
-        <v>6794</v>
-      </c>
-      <c r="B71" t="s">
-        <v>6795</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
-        <v>6796</v>
-      </c>
-      <c r="B72" t="s">
-        <v>6797</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
-        <v>2571</v>
-      </c>
-      <c r="B73" t="s">
-        <v>6798</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
-        <v>5656</v>
-      </c>
-      <c r="B74" t="s">
-        <v>5163</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
-        <v>6799</v>
-      </c>
-      <c r="B75" t="s">
-        <v>6364</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
-        <v>6161</v>
-      </c>
-      <c r="B76" t="s">
-        <v>6800</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>5928</v>
-      </c>
-      <c r="B77" t="s">
-        <v>6801</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
-        <v>6802</v>
-      </c>
-      <c r="B78" t="s">
-        <v>6803</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
-        <v>3467</v>
-      </c>
-      <c r="B79" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
-        <v>6804</v>
-      </c>
-      <c r="B80" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
-        <v>6805</v>
-      </c>
-      <c r="B81" t="s">
-        <v>6806</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
-        <v>6807</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6808</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
-        <v>6809</v>
-      </c>
-      <c r="B83" t="s">
-        <v>6810</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>6811</v>
-      </c>
-      <c r="B84" t="s">
-        <v>6812</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>6813</v>
-      </c>
-      <c r="B85" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>2323</v>
-      </c>
-      <c r="B86" t="s">
-        <v>6814</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
-        <v>6815</v>
-      </c>
-      <c r="B87" t="s">
-        <v>6816</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
-        <v>6817</v>
-      </c>
-      <c r="B88" t="s">
-        <v>6818</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>6819</v>
-      </c>
-      <c r="B89" t="s">
-        <v>6820</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B90" t="s">
-        <v>6821</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B91" t="s">
-        <v>6822</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>2331</v>
-      </c>
-      <c r="B92" t="s">
-        <v>6624</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>2021</v>
-      </c>
-      <c r="B93" t="s">
-        <v>5683</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>6823</v>
-      </c>
-      <c r="B94" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
-        <v>5209</v>
-      </c>
-      <c r="B95" t="s">
-        <v>1997</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>6824</v>
-      </c>
-      <c r="B96" t="s">
-        <v>6825</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
-        <v>6826</v>
-      </c>
-      <c r="B97" t="s">
-        <v>6827</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
-        <v>6828</v>
-      </c>
-      <c r="B98" t="s">
-        <v>6829</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
-        <v>6830</v>
-      </c>
-      <c r="B99" t="s">
-        <v>6831</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
-        <v>6832</v>
-      </c>
-      <c r="B100" t="s">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
-        <v>6833</v>
-      </c>
-      <c r="B101" t="s">
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B102" t="s">
-        <v>5457</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" t="s">
-        <v>6834</v>
-      </c>
-      <c r="B103" t="s">
-        <v>6835</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
-        <v>6836</v>
-      </c>
-      <c r="B104" t="s">
-        <v>2330</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
-        <v>228</v>
-      </c>
-      <c r="B105" t="s">
-        <v>6837</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" t="s">
-        <v>1355</v>
-      </c>
-      <c r="B106" t="s">
-        <v>2333</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
-        <v>2355</v>
-      </c>
-      <c r="B107" t="s">
-        <v>6838</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
-        <v>6839</v>
-      </c>
-      <c r="B108" t="s">
-        <v>6840</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
-        <v>1678</v>
-      </c>
-      <c r="B109" t="s">
-        <v>6841</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B110" t="s">
-        <v>6842</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B111" t="s">
-        <v>6843</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" t="s">
-        <v>5470</v>
-      </c>
-      <c r="B112" t="s">
-        <v>6844</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" t="s">
-        <v>5471</v>
-      </c>
-      <c r="B113" t="s">
-        <v>6845</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" t="s">
-        <v>6846</v>
-      </c>
-      <c r="B114" t="s">
-        <v>6847</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" t="s">
-        <v>3836</v>
-      </c>
-      <c r="B115" t="s">
-        <v>6848</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" t="s">
-        <v>2371</v>
-      </c>
-      <c r="B116" t="s">
-        <v>6849</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" t="s">
-        <v>2373</v>
-      </c>
-      <c r="B117" t="s">
-        <v>6850</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" t="s">
-        <v>5478</v>
-      </c>
-      <c r="B118" t="s">
-        <v>6205</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" t="s">
-        <v>6851</v>
-      </c>
-      <c r="B119" t="s">
-        <v>6852</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" t="s">
-        <v>6853</v>
-      </c>
-      <c r="B120" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" t="s">
-        <v>2060</v>
-      </c>
-      <c r="B121" t="s">
-        <v>6854</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" t="s">
-        <v>6855</v>
-      </c>
-      <c r="B122" t="s">
-        <v>6856</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" t="s">
-        <v>6857</v>
-      </c>
-      <c r="B123" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" t="s">
-        <v>3245</v>
-      </c>
-      <c r="B124" t="s">
-        <v>6858</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" t="s">
-        <v>3247</v>
-      </c>
-      <c r="B125" t="s">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" t="s">
-        <v>2389</v>
-      </c>
-      <c r="B126" t="s">
-        <v>6859</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" t="s">
-        <v>2391</v>
-      </c>
-      <c r="B127" t="s">
-        <v>4403</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" t="s">
-        <v>3250</v>
-      </c>
-      <c r="B128" t="s">
-        <v>6860</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" t="s">
-        <v>3252</v>
-      </c>
-      <c r="B129" t="s">
-        <v>6861</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" t="s">
-        <v>3253</v>
-      </c>
-      <c r="B130" t="s">
-        <v>6862</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" t="s">
-        <v>3255</v>
-      </c>
-      <c r="B131" t="s">
-        <v>6863</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" t="s">
-        <v>5493</v>
-      </c>
-      <c r="B132" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" t="s">
-        <v>6864</v>
-      </c>
-      <c r="B133" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" t="s">
-        <v>6865</v>
-      </c>
-      <c r="B134" t="s">
-        <v>6866</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" t="s">
-        <v>5496</v>
-      </c>
-      <c r="B135" t="s">
-        <v>6867</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" t="s">
-        <v>6679</v>
-      </c>
-      <c r="B136" t="s">
-        <v>6868</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" t="s">
-        <v>6680</v>
-      </c>
-      <c r="B137" t="s">
-        <v>6869</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" t="s">
-        <v>5501</v>
-      </c>
-      <c r="B138" t="s">
-        <v>6870</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" t="s">
-        <v>5502</v>
-      </c>
-      <c r="B139" t="s">
-        <v>6871</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" t="s">
-        <v>5504</v>
-      </c>
-      <c r="B140" t="s">
-        <v>4725</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" t="s">
-        <v>6872</v>
-      </c>
-      <c r="B141" t="s">
-        <v>6873</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" t="s">
-        <v>6874</v>
-      </c>
-      <c r="B142" t="s">
-        <v>4728</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" t="s">
-        <v>4729</v>
-      </c>
-      <c r="B143" t="s">
-        <v>6875</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" t="s">
-        <v>6876</v>
-      </c>
-      <c r="B144" t="s">
-        <v>6877</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" t="s">
-        <v>5510</v>
-      </c>
-      <c r="B145" t="s">
-        <v>6878</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" t="s">
-        <v>6879</v>
-      </c>
-      <c r="B146" t="s">
-        <v>4735</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" t="s">
-        <v>5514</v>
-      </c>
-      <c r="B147" t="s">
-        <v>6880</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148" t="s">
-        <v>6881</v>
-      </c>
-      <c r="B148" t="s">
-        <v>6882</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" t="s">
-        <v>6883</v>
-      </c>
-      <c r="B149" t="s">
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" t="s">
-        <v>2425</v>
-      </c>
-      <c r="B150" t="s">
-        <v>6884</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" t="s">
-        <v>6885</v>
-      </c>
-      <c r="B151" t="s">
-        <v>6886</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" t="s">
-        <v>6887</v>
-      </c>
-      <c r="B152" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" t="s">
-        <v>6888</v>
-      </c>
-      <c r="B153" t="s">
-        <v>6889</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" t="s">
-        <v>6890</v>
-      </c>
-      <c r="B154" t="s">
-        <v>6891</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" t="s">
-        <v>6892</v>
-      </c>
-      <c r="B155" t="s">
-        <v>6488</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" t="s">
-        <v>6893</v>
-      </c>
-      <c r="B156" t="s">
-        <v>6894</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" t="s">
-        <v>6895</v>
-      </c>
-      <c r="B157" t="s">
-        <v>6896</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158" t="s">
-        <v>6897</v>
-      </c>
-      <c r="B158" t="s">
-        <v>2133</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" t="s">
-        <v>312</v>
-      </c>
-      <c r="B159" t="s">
-        <v>6898</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" t="s">
-        <v>2440</v>
-      </c>
-      <c r="B160" t="s">
-        <v>6899</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" t="s">
-        <v>6900</v>
-      </c>
-      <c r="B161" t="s">
-        <v>6499</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" t="s">
-        <v>6901</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" t="s">
-        <v>6902</v>
-      </c>
-      <c r="B163" t="s">
-        <v>6903</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164" t="s">
-        <v>4760</v>
-      </c>
-      <c r="B164" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2">
-      <c r="A165" t="s">
-        <v>6904</v>
-      </c>
-      <c r="B165" t="s">
-        <v>6280</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2">
-      <c r="A166" t="s">
-        <v>5302</v>
-      </c>
-      <c r="B166" t="s">
-        <v>5322</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2">
-      <c r="A167" t="s">
-        <v>6905</v>
-      </c>
-      <c r="B167" t="s">
-        <v>5324</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2">
-      <c r="A168" t="s">
-        <v>6906</v>
-      </c>
-      <c r="B168" t="s">
-        <v>6907</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2">
-      <c r="A169" t="s">
-        <v>6908</v>
-      </c>
-      <c r="B169" t="s">
-        <v>6909</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2">
-      <c r="A170" t="s">
-        <v>6910</v>
-      </c>
-      <c r="B170" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2">
-      <c r="A171" t="s">
-        <v>6911</v>
-      </c>
-      <c r="B171" t="s">
-        <v>3934</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2">
-      <c r="A172" t="s">
-        <v>6912</v>
-      </c>
-      <c r="B172" t="s">
-        <v>5058</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2">
-      <c r="A173" t="s">
-        <v>6913</v>
-      </c>
-      <c r="B173" t="s">
-        <v>6056</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2">
-      <c r="A174" t="s">
-        <v>6914</v>
-      </c>
-      <c r="B174" t="s">
-        <v>2764</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2">
-      <c r="A175" t="s">
-        <v>6915</v>
-      </c>
-      <c r="B175" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2">
-      <c r="A176" t="s">
-        <v>6916</v>
-      </c>
-      <c r="B176" t="s">
-        <v>6917</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2">
-      <c r="A177" t="s">
-        <v>6918</v>
-      </c>
-      <c r="B177" t="s">
-        <v>2172</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2">
-      <c r="A178" t="s">
-        <v>2468</v>
-      </c>
-      <c r="B178" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2">
-      <c r="A179" t="s">
-        <v>6919</v>
-      </c>
-      <c r="B179" t="s">
-        <v>4783</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2">
-      <c r="A180" t="s">
-        <v>2471</v>
-      </c>
-      <c r="B180" t="s">
-        <v>6920</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2">
-      <c r="A181" t="s">
-        <v>6921</v>
-      </c>
-      <c r="B181" t="s">
-        <v>2458</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
-      <c r="A182" t="s">
-        <v>6922</v>
-      </c>
-      <c r="B182" t="s">
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2">
-      <c r="A183" t="s">
-        <v>6923</v>
-      </c>
-      <c r="B183" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2">
-      <c r="A184" t="s">
-        <v>2476</v>
-      </c>
-      <c r="B184" t="s">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2">
-      <c r="A185" t="s">
-        <v>6924</v>
-      </c>
-      <c r="B185" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2">
-      <c r="A186" t="s">
-        <v>2478</v>
-      </c>
-      <c r="B186" t="s">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2">
-      <c r="A187" t="s">
-        <v>2479</v>
-      </c>
-      <c r="B187" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2">
-      <c r="A188" t="s">
-        <v>6925</v>
-      </c>
-      <c r="B188" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2">
-      <c r="A189" t="s">
-        <v>2480</v>
-      </c>
-      <c r="B189" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2">
-      <c r="A190" t="s">
-        <v>6926</v>
-      </c>
-      <c r="B190" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2">
-      <c r="A191" t="s">
-        <v>6927</v>
-      </c>
-      <c r="B191" t="s">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2">
-      <c r="A192" t="s">
-        <v>2177</v>
-      </c>
-      <c r="B192" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2">
-      <c r="A193" t="s">
-        <v>3652</v>
-      </c>
-      <c r="B193" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2">
-      <c r="A194" t="s">
-        <v>6928</v>
-      </c>
-      <c r="B194" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2">
-      <c r="A195" t="s">
-        <v>6929</v>
-      </c>
-      <c r="B195" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2">
-      <c r="A196" t="s">
-        <v>4793</v>
-      </c>
-      <c r="B196" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2">
-      <c r="A197" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B197" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2">
-      <c r="A198" t="s">
-        <v>5824</v>
-      </c>
-      <c r="B198" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2">
-      <c r="A199" t="s">
-        <v>1840</v>
-      </c>
-      <c r="B199" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2">
-      <c r="A200" t="s">
-        <v>1841</v>
-      </c>
-      <c r="B200" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2">
-      <c r="A201" t="s">
-        <v>785</v>
-      </c>
-      <c r="B201" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2">
-      <c r="A202" t="s">
-        <v>787</v>
-      </c>
-      <c r="B202" t="s">
-        <v>401</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>